<commit_message>
adding header detection improvement by usid bold format to find the header and also restrict on sheet that not what we want.
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JLFHLZN.xlsx
+++ b/invoice_gen/TEMPLATE/JLFHLZN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\tools\inv_pkl_contract_creation - Copy\invoice_gen\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\project\generated_shippinglist_invoice\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0433ED21-3680-46C0-BB79-FC28BCA224FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24CA88F-F10A-407F-A34D-EC564A10C11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="10" r:id="rId1"/>
@@ -75,21 +75,12 @@
     <t xml:space="preserve">HIGH LINE SMART HOME VIETNAM CO., LTD  </t>
   </si>
   <si>
-    <t xml:space="preserve">Lot F5, D4 Street, Minh Hung III Industrial Park   </t>
-  </si>
-  <si>
     <t xml:space="preserve">XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, </t>
   </si>
   <si>
-    <t>Minh Hung Commune, Chon Thanh District</t>
-  </si>
-  <si>
     <t>Prey Kokir  Commune, Chantrea District,</t>
   </si>
   <si>
-    <t>Binh Phuoc Province,Vietnam</t>
-  </si>
-  <si>
     <t>Kingdom of Cambodia.</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
   </si>
   <si>
     <t>Deliver Date &amp; of Transportation</t>
-  </si>
-  <si>
-    <t>NO LATER THAN MAY 31. 2025 BY TRUCK</t>
   </si>
   <si>
     <t>Port of Loading:</t>
@@ -167,7 +155,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>BENEFICIARY BANK</t>
     </r>
@@ -185,7 +173,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH /BANK OF CHINA PHNOM PENH BRANCH</t>
     </r>
@@ -254,12 +242,6 @@
     <t>HIGH LINE SMART HOME VIETNAM CO.,LTD.</t>
   </si>
   <si>
-    <t>LOT F5, D4 STREET, MINH HUNG III INDUSTRIAL PARK, MINH HUNG WARD,</t>
-  </si>
-  <si>
-    <t>CHON THANH TOWN, BINH PHUOC PROVINCE, VIETNAM</t>
-  </si>
-  <si>
     <t>EMAIL:import@highlinesmart.com</t>
   </si>
   <si>
@@ -267,9 +249,6 @@
   </si>
   <si>
     <t xml:space="preserve">SHIP: </t>
-  </si>
-  <si>
-    <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO BINH PHUOC PROVINCE, VIETNAM.</t>
   </si>
   <si>
     <t xml:space="preserve">Country of Original Cambodia </t>
@@ -287,7 +266,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>BENEFICIARY BANK</t>
     </r>
@@ -305,7 +284,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH/BANK OF CHINA PHNOM PENH BRANCH</t>
     </r>
@@ -319,7 +298,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">SWIFT CODE  </t>
     </r>
@@ -337,7 +316,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>BKCHKHPPXXX</t>
     </r>
@@ -363,7 +342,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>BENEFICIARY BANK</t>
     </r>
@@ -381,7 +360,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH /BANK OF CHINA PHNOM PENH BRANCH</t>
     </r>
@@ -392,7 +371,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">SWIFT CODE  </t>
     </r>
@@ -401,7 +380,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>：BKCHKHPPXXX</t>
     </r>
@@ -414,19 +393,41 @@
   </si>
   <si>
     <t>JFINV</t>
+  </si>
+  <si>
+    <t>Lot F5, D4 street, Minh Hung III Industrial Park,</t>
+  </si>
+  <si>
+    <t>Minh Hung Ward, Dong Nai Province, Vietnam</t>
+  </si>
+  <si>
+    <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lot F5, D4 street, Minh Hung III Industrial Park,  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minh Hung Ward, Dong Nai Province, </t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>NO LATER THAN November 5, 2025 BY TRUCK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
     <numFmt numFmtId="166" formatCode="d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0.00_ ;_-&quot;$&quot;* \-#,##0.00\ ;_-&quot;$&quot;* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="169" formatCode="0.0_);[Red]\(0.0\)"/>
+    <numFmt numFmtId="170" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -440,33 +441,33 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -474,33 +475,33 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Book Antiqua"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -508,60 +509,54 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Book Antiqua"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -574,18 +569,18 @@
       <b/>
       <sz val="20"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -595,7 +590,7 @@
     <font>
       <sz val="14"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -613,7 +608,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -654,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -733,26 +734,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -763,21 +755,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -786,15 +778,25 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,9 +806,36 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -816,30 +845,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1401,37 +1408,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="36" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="36" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="36" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="36"/>
-    <col min="8" max="16384" width="7.5703125" style="36"/>
+    <col min="1" max="1" width="22.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="33" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="33" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="33"/>
+    <col min="8" max="9" width="7.5703125" style="33"/>
+    <col min="10" max="10" width="26.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="7.5703125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="35" customFormat="1" ht="38.25" customHeight="1">
+    <row r="1" spans="1:8" s="32" customFormat="1" ht="38.25" customHeight="1">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-    </row>
-    <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="56" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" s="32" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="56"/>
@@ -1439,23 +1448,23 @@
       <c r="D2" s="56"/>
       <c r="E2" s="56"/>
       <c r="F2" s="56"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-    </row>
-    <row r="3" spans="1:8" s="35" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A3" s="57" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:8" s="32" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-    </row>
-    <row r="4" spans="1:8" s="35" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="1:8" s="32" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="56"/>
@@ -1463,23 +1472,23 @@
       <c r="D4" s="56"/>
       <c r="E4" s="56"/>
       <c r="F4" s="56"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-    </row>
-    <row r="5" spans="1:8" s="35" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A5" s="58" t="s">
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:8" s="32" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A5" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" ht="27" customHeight="1">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="53"/>
@@ -1489,374 +1498,369 @@
       <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="37"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="F17" s="37"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="40"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40" t="s">
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+    </row>
+    <row r="27" spans="1:10" ht="18.75">
+      <c r="A27" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="40"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="42"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="43"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="40" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+    </row>
+    <row r="29" spans="1:10" ht="26.1" customHeight="1">
+      <c r="A29" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="40"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="40" t="s">
+      <c r="B29" s="54" t="s">
         <v>32</v>
-      </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-    </row>
-    <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="45"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-    </row>
-    <row r="29" spans="1:8" ht="26.1" customHeight="1">
-      <c r="A29" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="54" t="s">
-        <v>36</v>
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="54"/>
       <c r="E29" s="54"/>
       <c r="F29" s="54"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-    </row>
-    <row r="31" spans="1:8" ht="27" customHeight="1">
-      <c r="A31" s="40" t="s">
-        <v>39</v>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="J29" s="50"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+    </row>
+    <row r="31" spans="1:10" ht="27" customHeight="1">
+      <c r="A31" s="37" t="s">
+        <v>35</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>
       <c r="E31" s="54"/>
       <c r="F31" s="54"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="49"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75">
-      <c r="A32" s="40" t="s">
+      <c r="G31" s="45"/>
+      <c r="H31" s="46"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75">
+      <c r="A32" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="46"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75">
+      <c r="A33" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="46"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75">
+      <c r="A34" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="46"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="49"/>
-    </row>
-    <row r="33" spans="1:8" ht="15.75">
-      <c r="A33" s="40" t="s">
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="49"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75">
-      <c r="A34" s="40" t="s">
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+    </row>
+    <row r="38" spans="1:8" ht="48.75" customHeight="1">
+      <c r="A38" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="49"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="40" t="s">
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-    </row>
-    <row r="38" spans="1:8" ht="48.75" customHeight="1">
-      <c r="A38" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1882,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="15"/>
@@ -1902,70 +1906,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="71"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="71"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="71"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="71"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
     </row>
     <row r="6" spans="1:7" ht="83.25" customHeight="1">
-      <c r="A6" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
+      <c r="A6" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="5"/>
@@ -1974,51 +1978,51 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>83</v>
+      <c r="E8" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="69"/>
+      <c r="G8" s="26" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="22.5" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.25" customHeight="1">
@@ -2041,10 +2045,10 @@
     </row>
     <row r="13" spans="1:7" ht="25.5" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -2053,8 +2057,8 @@
     </row>
     <row r="14" spans="1:7" ht="25.5" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="65" t="s">
-        <v>62</v>
+      <c r="B14" s="64" t="s">
+        <v>77</v>
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="65"/>
@@ -2064,7 +2068,7 @@
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="14" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -2074,23 +2078,23 @@
     <row r="16" spans="1:7" ht="24" customHeight="1">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="26.1" customHeight="1">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="27.75" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -2104,21 +2108,21 @@
     </row>
     <row r="21" spans="1:7" ht="42" customHeight="1">
       <c r="A21" s="66" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B21" s="66"/>
       <c r="C21" s="66"/>
       <c r="D21" s="18"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="33"/>
+      <c r="G21" s="30"/>
     </row>
     <row r="22" spans="1:7" ht="61.5" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B22" s="67" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C22" s="67"/>
       <c r="D22" s="20"/>
@@ -2128,7 +2132,7 @@
     </row>
     <row r="23" spans="1:7" ht="33.950000000000003" customHeight="1">
       <c r="A23" s="68" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B23" s="68"/>
       <c r="C23" s="68"/>
@@ -2138,26 +2142,26 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A24" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
+      <c r="A24" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="A25" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
+      <c r="A25" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
     </row>
     <row r="26" spans="1:7" ht="42" customHeight="1">
       <c r="E26" s="29"/>
@@ -2169,7 +2173,7 @@
     <row r="27" spans="1:7" ht="24" customHeight="1">
       <c r="E27" s="5"/>
       <c r="F27" s="23" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="69.75" customHeight="1">
@@ -2182,8 +2186,8 @@
     </row>
     <row r="30" spans="1:7" ht="53.1" customHeight="1">
       <c r="E30" s="5"/>
-      <c r="F30" s="34" t="s">
-        <v>75</v>
+      <c r="F30" s="31" t="s">
+        <v>68</v>
       </c>
       <c r="G30" s="6"/>
     </row>
@@ -2208,7 +2212,12 @@
     <row r="49" ht="17.25" customHeight="1"/>
     <row r="61" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A24:G24"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A6:G6"/>
@@ -2216,11 +2225,7 @@
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="J21:J33">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -2236,8 +2241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="15"/>
@@ -2257,92 +2262,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="71"/>
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="24" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="71"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="71"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" ht="54" customHeight="1">
-      <c r="A6" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
+      <c r="A6" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
     </row>
@@ -2355,56 +2360,55 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="71"/>
+      <c r="G8" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="69"/>
       <c r="I8" s="26" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="22.5" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="29"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="20.25" customHeight="1">
       <c r="A11" s="5"/>
@@ -2433,10 +2437,10 @@
     </row>
     <row r="13" spans="1:11" ht="25.5" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -2447,8 +2451,8 @@
     </row>
     <row r="14" spans="1:11" ht="25.5" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="65" t="s">
-        <v>62</v>
+      <c r="B14" s="64" t="s">
+        <v>77</v>
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="65"/>
@@ -2460,7 +2464,7 @@
     <row r="15" spans="1:11" ht="25.5" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="14" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -2472,7 +2476,7 @@
     <row r="16" spans="1:11" ht="24" customHeight="1">
       <c r="A16" s="16"/>
       <c r="B16" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -2481,7 +2485,7 @@
     <row r="17" spans="1:12" ht="26.1" customHeight="1">
       <c r="A17" s="16"/>
       <c r="B17" s="14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -2489,10 +2493,10 @@
     </row>
     <row r="18" spans="1:12" ht="27.75" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -2508,7 +2512,7 @@
     </row>
     <row r="21" spans="1:12" ht="48" customHeight="1">
       <c r="A21" s="66" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B21" s="66"/>
       <c r="C21" s="66"/>
@@ -2524,10 +2528,10 @@
     </row>
     <row r="22" spans="1:12" ht="72" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B22" s="67" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C22" s="67"/>
       <c r="D22" s="20"/>
@@ -2542,7 +2546,7 @@
     </row>
     <row r="23" spans="1:12" ht="42" customHeight="1">
       <c r="A23" s="68" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B23" s="68"/>
       <c r="C23" s="68"/>
@@ -2557,34 +2561,34 @@
       <c r="L23" s="10"/>
     </row>
     <row r="24" spans="1:12" ht="48" customHeight="1">
-      <c r="A24" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
+      <c r="A24" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" ht="48" customHeight="1">
-      <c r="A25" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="63"/>
+      <c r="A25" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
     </row>
     <row r="26" spans="1:12" ht="42" customHeight="1">
       <c r="F26" s="5"/>
@@ -2608,8 +2612,8 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="J29" s="70"/>
-      <c r="K29" s="70"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="65"/>
     </row>
     <row r="30" spans="1:12" ht="53.1" customHeight="1">
       <c r="F30" s="5"/>
@@ -2640,13 +2644,8 @@
     <row r="61" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="G8:H8"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A1:I1"/>
@@ -2654,6 +2653,11 @@
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:I5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <conditionalFormatting sqref="N21:N33">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>

</xml_diff>